<commit_message>
WIP - update filter, insert, import UI
</commit_message>
<xml_diff>
--- a/public/Electrics201904.xlsx
+++ b/public/Electrics201904.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\LaravelProject\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1FDB1D-9928-4164-A85F-632D7C84F365}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC67F12-602D-4EDE-8BFF-A9F62C9EA178}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BEE16C92-69ED-4BA2-852C-5F74E3486C55}"/>
   </bookViews>
@@ -50,10 +50,10 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Deleted</t>
+    <t>2019-04</t>
   </si>
   <si>
-    <t>2019-04</t>
+    <t>Room</t>
   </si>
 </sst>
 </file>
@@ -62,7 +62,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -106,7 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -426,19 +426,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F47461D-A76F-4827-B3B8-BEE949F24345}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -446,42 +447,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="2">
+        <v>206</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>215</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>250</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>150000</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -491,20 +492,20 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="2">
+        <v>207</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
         <v>226</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>250</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>114000</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -514,20 +515,20 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="2">
+        <v>208</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
         <v>211</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>250</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>100000</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -537,20 +538,20 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="2">
+        <v>209</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
         <v>25</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>55</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>97000</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -560,20 +561,20 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="2">
+        <v>210</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
         <v>111</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>124</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>111000</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -583,20 +584,20 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="2">
+        <v>211</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
         <v>242</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>255</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>315000</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -606,20 +607,20 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="2">
+        <v>212</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
         <v>112</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>151</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>144000</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -629,20 +630,20 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="2">
+        <v>306</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
         <v>222</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>252</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>157000</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -652,20 +653,20 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="2">
+        <v>307</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
         <v>21</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>61</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>151000</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -675,20 +676,20 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="2">
+        <v>308</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
         <v>221</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>255</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>250000</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>

</xml_diff>

<commit_message>
WIP - Update function insert new record electric
</commit_message>
<xml_diff>
--- a/public/Electrics201904.xlsx
+++ b/public/Electrics201904.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\LaravelProject\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC67F12-602D-4EDE-8BFF-A9F62C9EA178}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F8B9C4-9E64-492A-AFD3-7710CD7904B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BEE16C92-69ED-4BA2-852C-5F74E3486C55}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>RoomID</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Room</t>
+  </si>
+  <si>
+    <t>Bếp</t>
   </si>
 </sst>
 </file>
@@ -101,13 +104,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -424,15 +430,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F47461D-A76F-4827-B3B8-BEE949F24345}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" customWidth="1"/>
@@ -469,7 +475,7 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>206</v>
       </c>
       <c r="C2" t="s">
@@ -485,14 +491,14 @@
         <v>150000</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>207</v>
       </c>
       <c r="C3" t="s">
@@ -508,14 +514,14 @@
         <v>114000</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>208</v>
       </c>
       <c r="C4" t="s">
@@ -531,14 +537,14 @@
         <v>100000</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>209</v>
       </c>
       <c r="C5" t="s">
@@ -554,14 +560,14 @@
         <v>97000</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>210</v>
       </c>
       <c r="C6" t="s">
@@ -577,14 +583,14 @@
         <v>111000</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>211</v>
       </c>
       <c r="C7" t="s">
@@ -600,14 +606,14 @@
         <v>315000</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>212</v>
       </c>
       <c r="C8" t="s">
@@ -623,14 +629,14 @@
         <v>144000</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>306</v>
       </c>
       <c r="C9" t="s">
@@ -646,14 +652,14 @@
         <v>157000</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>307</v>
       </c>
       <c r="C10" t="s">
@@ -669,33 +675,57 @@
         <v>151000</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>308</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11">
-        <v>221</v>
+        <v>21</v>
       </c>
       <c r="E11">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="F11">
-        <v>250000</v>
+        <v>151000</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>1550</v>
+      </c>
+      <c r="E12">
+        <v>1705</v>
+      </c>
+      <c r="F12">
+        <v>365000</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>